<commit_message>
versie 0.3 van urenregistratie
</commit_message>
<xml_diff>
--- a/TI-1.4 1819-Scrum-tijdregistratie-v1.0.xlsx
+++ b/TI-1.4 1819-Scrum-tijdregistratie-v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi Vlasblom\Desktop\schooltroep\Avans Jaar 1\1.4\Proftaak\ProftaakA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6C3490-AE4F-4DF4-A660-279767EFCEE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A702A790-8917-47A8-8432-E9E4F063D5D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="103">
   <si>
     <t>analyse van de tijdens de sprint bestede tijd</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>Ties, Hanno</t>
+  </si>
+  <si>
+    <t>Pir-sensor Testen</t>
   </si>
 </sst>
 </file>
@@ -1388,6 +1391,12 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1406,6 +1415,30 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1448,28 +1481,52 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1478,64 +1535,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2255,9 +2258,9 @@
         <v>47</v>
       </c>
       <c r="C3" s="113"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="117"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="119"/>
     </row>
     <row r="4" spans="2:6" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="114"/>
@@ -2273,19 +2276,19 @@
       </c>
     </row>
     <row r="5" spans="2:6" s="1" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="118" t="s">
+      <c r="B5" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="119"/>
+      <c r="C5" s="121"/>
       <c r="D5" s="109"/>
       <c r="E5" s="109"/>
       <c r="F5" s="115"/>
     </row>
     <row r="6" spans="2:6" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="121"/>
+      <c r="C6" s="123"/>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
       <c r="F6" s="111"/>
@@ -2330,15 +2333,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="str">
@@ -2415,17 +2418,17 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="141"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="129"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -2438,40 +2441,40 @@
     </row>
     <row r="7" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="122" t="s">
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="124"/>
-      <c r="L8" s="122" t="s">
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="134"/>
+      <c r="L8" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="124"/>
-      <c r="S8" s="122" t="s">
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="134"/>
+      <c r="S8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="123"/>
-      <c r="U8" s="123"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="134"/>
     </row>
     <row r="9" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="143"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
@@ -4336,47 +4339,47 @@
       <c r="B36" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="125">
+      <c r="C36" s="135">
         <f>C35+E35</f>
         <v>45</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="126"/>
-      <c r="G36" s="127">
+      <c r="D36" s="135"/>
+      <c r="E36" s="136"/>
+      <c r="G36" s="137">
         <f>G35+I35</f>
         <v>7</v>
       </c>
-      <c r="H36" s="128"/>
-      <c r="I36" s="129"/>
-      <c r="L36" s="130">
+      <c r="H36" s="138"/>
+      <c r="I36" s="139"/>
+      <c r="L36" s="140">
         <f>SUM(L35:Q35)</f>
         <v>45</v>
       </c>
-      <c r="M36" s="131"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="131"/>
-      <c r="P36" s="131"/>
-      <c r="Q36" s="132"/>
-      <c r="S36" s="133">
+      <c r="M36" s="141"/>
+      <c r="N36" s="141"/>
+      <c r="O36" s="141"/>
+      <c r="P36" s="141"/>
+      <c r="Q36" s="142"/>
+      <c r="S36" s="143">
         <f>SUM(S35:X35)</f>
         <v>6</v>
       </c>
-      <c r="T36" s="134"/>
-      <c r="U36" s="134"/>
-      <c r="V36" s="134"/>
-      <c r="W36" s="134"/>
-      <c r="X36" s="135"/>
+      <c r="T36" s="144"/>
+      <c r="U36" s="144"/>
+      <c r="V36" s="144"/>
+      <c r="W36" s="144"/>
+      <c r="X36" s="145"/>
     </row>
     <row r="37" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="136">
+      <c r="C37" s="124">
         <f>C39*C40</f>
         <v>42</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="137"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
@@ -4424,18 +4427,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S8:X8"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="L36:Q36"/>
+    <mergeCell ref="S36:X36"/>
+    <mergeCell ref="L8:Q8"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="S8:X8"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="L36:Q36"/>
-    <mergeCell ref="S36:X36"/>
-    <mergeCell ref="L8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="C17:C34 C10:C15">
     <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
@@ -4509,15 +4512,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B2" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
+      <c r="B2" s="162" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="54" t="str">
@@ -4594,17 +4597,17 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="146"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="146"/>
-      <c r="J6" s="147"/>
+      <c r="C6" s="157"/>
+      <c r="D6" s="157"/>
+      <c r="E6" s="157"/>
+      <c r="F6" s="157"/>
+      <c r="G6" s="157"/>
+      <c r="H6" s="157"/>
+      <c r="I6" s="157"/>
+      <c r="J6" s="158"/>
       <c r="L6" s="53"/>
       <c r="M6" s="53"/>
       <c r="N6" s="53"/>
@@ -4617,40 +4620,40 @@
     </row>
     <row r="7" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:24" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="148" t="s">
+      <c r="B8" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="150" t="s">
+      <c r="C8" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="151"/>
-      <c r="E8" s="151"/>
-      <c r="F8" s="152"/>
-      <c r="G8" s="150" t="s">
+      <c r="D8" s="147"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="148"/>
+      <c r="G8" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="151"/>
-      <c r="I8" s="151"/>
-      <c r="J8" s="152"/>
-      <c r="L8" s="150" t="s">
+      <c r="H8" s="147"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="148"/>
+      <c r="L8" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="151"/>
-      <c r="N8" s="151"/>
-      <c r="O8" s="151"/>
-      <c r="P8" s="151"/>
-      <c r="Q8" s="152"/>
-      <c r="S8" s="150" t="s">
+      <c r="M8" s="147"/>
+      <c r="N8" s="147"/>
+      <c r="O8" s="147"/>
+      <c r="P8" s="147"/>
+      <c r="Q8" s="148"/>
+      <c r="S8" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="151"/>
-      <c r="U8" s="151"/>
-      <c r="V8" s="151"/>
-      <c r="W8" s="151"/>
-      <c r="X8" s="152"/>
+      <c r="T8" s="147"/>
+      <c r="U8" s="147"/>
+      <c r="V8" s="147"/>
+      <c r="W8" s="147"/>
+      <c r="X8" s="148"/>
     </row>
     <row r="9" spans="2:24" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="149"/>
+      <c r="B9" s="165"/>
       <c r="C9" s="60" t="s">
         <v>2</v>
       </c>
@@ -6551,47 +6554,47 @@
       <c r="B36" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="153">
+      <c r="C36" s="149">
         <f>C35+E35</f>
         <v>41.25</v>
       </c>
-      <c r="D36" s="153"/>
-      <c r="E36" s="154"/>
-      <c r="G36" s="161">
+      <c r="D36" s="149"/>
+      <c r="E36" s="150"/>
+      <c r="G36" s="159">
         <f>G35+I35</f>
         <v>18.2</v>
       </c>
-      <c r="H36" s="162"/>
-      <c r="I36" s="163"/>
-      <c r="L36" s="157">
+      <c r="H36" s="160"/>
+      <c r="I36" s="161"/>
+      <c r="L36" s="153">
         <f>SUM(L35:Q35)</f>
         <v>27.25</v>
       </c>
-      <c r="M36" s="158"/>
-      <c r="N36" s="158"/>
-      <c r="O36" s="158"/>
-      <c r="P36" s="158"/>
-      <c r="Q36" s="159"/>
-      <c r="S36" s="160">
+      <c r="M36" s="154"/>
+      <c r="N36" s="154"/>
+      <c r="O36" s="154"/>
+      <c r="P36" s="154"/>
+      <c r="Q36" s="155"/>
+      <c r="S36" s="156">
         <f>SUM(S35:X35)</f>
         <v>18.2</v>
       </c>
-      <c r="T36" s="146"/>
-      <c r="U36" s="146"/>
-      <c r="V36" s="146"/>
-      <c r="W36" s="146"/>
-      <c r="X36" s="147"/>
+      <c r="T36" s="157"/>
+      <c r="U36" s="157"/>
+      <c r="V36" s="157"/>
+      <c r="W36" s="157"/>
+      <c r="X36" s="158"/>
     </row>
     <row r="37" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="155">
+      <c r="C37" s="151">
         <f>C39*C40</f>
         <v>42</v>
       </c>
-      <c r="D37" s="155"/>
-      <c r="E37" s="156"/>
+      <c r="D37" s="151"/>
+      <c r="E37" s="152"/>
       <c r="F37" s="53"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
@@ -6639,6 +6642,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:J8"/>
     <mergeCell ref="S8:X8"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
@@ -6646,11 +6654,6 @@
     <mergeCell ref="S36:X36"/>
     <mergeCell ref="G36:I36"/>
     <mergeCell ref="L8:Q8"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C34">
     <cfRule type="cellIs" dxfId="37" priority="7" operator="greaterThan">
@@ -6694,10 +6697,10 @@
   <dimension ref="B2:X42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B22" activeCellId="2" sqref="B20 B21 B22"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6715,15 +6718,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="str">
@@ -6800,17 +6803,17 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="141"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="129"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -6823,40 +6826,40 @@
     </row>
     <row r="7" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="122" t="s">
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="124"/>
-      <c r="L8" s="122" t="s">
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="134"/>
+      <c r="L8" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="124"/>
-      <c r="S8" s="122" t="s">
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="134"/>
+      <c r="S8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="123"/>
-      <c r="U8" s="123"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="134"/>
     </row>
     <row r="9" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="143"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
@@ -8719,47 +8722,47 @@
       <c r="B36" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="125">
+      <c r="C36" s="135">
         <f>C35+E35</f>
         <v>45</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="126"/>
-      <c r="G36" s="127">
+      <c r="D36" s="135"/>
+      <c r="E36" s="136"/>
+      <c r="G36" s="137">
         <f>G35+I35</f>
         <v>6</v>
       </c>
-      <c r="H36" s="128"/>
-      <c r="I36" s="129"/>
-      <c r="L36" s="130">
+      <c r="H36" s="138"/>
+      <c r="I36" s="139"/>
+      <c r="L36" s="140">
         <f>SUM(L35:Q35)</f>
         <v>45</v>
       </c>
-      <c r="M36" s="131"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="131"/>
-      <c r="P36" s="131"/>
-      <c r="Q36" s="132"/>
-      <c r="S36" s="133">
+      <c r="M36" s="141"/>
+      <c r="N36" s="141"/>
+      <c r="O36" s="141"/>
+      <c r="P36" s="141"/>
+      <c r="Q36" s="142"/>
+      <c r="S36" s="143">
         <f>SUM(S35:X35)</f>
         <v>6</v>
       </c>
-      <c r="T36" s="134"/>
-      <c r="U36" s="134"/>
-      <c r="V36" s="134"/>
-      <c r="W36" s="134"/>
-      <c r="X36" s="135"/>
+      <c r="T36" s="144"/>
+      <c r="U36" s="144"/>
+      <c r="V36" s="144"/>
+      <c r="W36" s="144"/>
+      <c r="X36" s="145"/>
     </row>
     <row r="37" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="136">
+      <c r="C37" s="124">
         <f>C39*C40</f>
         <v>42</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="137"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
@@ -8807,18 +8810,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S8:X8"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="L36:Q36"/>
+    <mergeCell ref="S36:X36"/>
+    <mergeCell ref="L8:Q8"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="S8:X8"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="L36:Q36"/>
-    <mergeCell ref="S36:X36"/>
-    <mergeCell ref="L8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="C28:C34">
     <cfRule type="cellIs" dxfId="30" priority="9" operator="greaterThan">
@@ -8893,15 +8896,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="str">
@@ -8978,17 +8981,17 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="141"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="129"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -9001,40 +9004,40 @@
     </row>
     <row r="7" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="122" t="s">
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="124"/>
-      <c r="L8" s="122" t="s">
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="134"/>
+      <c r="L8" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="124"/>
-      <c r="S8" s="122" t="s">
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="134"/>
+      <c r="S8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="123"/>
-      <c r="U8" s="123"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="134"/>
     </row>
     <row r="9" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="143"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
@@ -9121,7 +9124,7 @@
       <c r="H10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="164"/>
+      <c r="I10" s="116"/>
       <c r="J10" s="21" t="s">
         <v>71</v>
       </c>
@@ -9193,7 +9196,7 @@
       <c r="H11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I11" s="164"/>
+      <c r="I11" s="116"/>
       <c r="J11" s="21" t="s">
         <v>72</v>
       </c>
@@ -9269,7 +9272,7 @@
       <c r="H12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="164">
+      <c r="I12" s="116">
         <v>1</v>
       </c>
       <c r="J12" s="21" t="s">
@@ -9343,7 +9346,7 @@
       <c r="H13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="164"/>
+      <c r="I13" s="116"/>
       <c r="J13" s="21" t="s">
         <v>69</v>
       </c>
@@ -9415,7 +9418,7 @@
       <c r="H14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="164"/>
+      <c r="I14" s="116"/>
       <c r="J14" s="21" t="s">
         <v>82</v>
       </c>
@@ -10785,47 +10788,47 @@
       <c r="B36" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="125">
+      <c r="C36" s="135">
         <f>C35+E35</f>
         <v>6.25</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="126"/>
-      <c r="G36" s="127">
+      <c r="D36" s="135"/>
+      <c r="E36" s="136"/>
+      <c r="G36" s="137">
         <f>G35+I35</f>
         <v>6</v>
       </c>
-      <c r="H36" s="128"/>
-      <c r="I36" s="129"/>
-      <c r="L36" s="130">
+      <c r="H36" s="138"/>
+      <c r="I36" s="139"/>
+      <c r="L36" s="140">
         <f>SUM(L35:Q35)</f>
         <v>1.25</v>
       </c>
-      <c r="M36" s="131"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="131"/>
-      <c r="P36" s="131"/>
-      <c r="Q36" s="132"/>
-      <c r="S36" s="133">
+      <c r="M36" s="141"/>
+      <c r="N36" s="141"/>
+      <c r="O36" s="141"/>
+      <c r="P36" s="141"/>
+      <c r="Q36" s="142"/>
+      <c r="S36" s="143">
         <f>SUM(S35:X35)</f>
         <v>1</v>
       </c>
-      <c r="T36" s="134"/>
-      <c r="U36" s="134"/>
-      <c r="V36" s="134"/>
-      <c r="W36" s="134"/>
-      <c r="X36" s="135"/>
+      <c r="T36" s="144"/>
+      <c r="U36" s="144"/>
+      <c r="V36" s="144"/>
+      <c r="W36" s="144"/>
+      <c r="X36" s="145"/>
     </row>
     <row r="37" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="136">
+      <c r="C37" s="124">
         <f>C39*C40</f>
         <v>42</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="137"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
@@ -10873,18 +10876,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S8:X8"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="L36:Q36"/>
+    <mergeCell ref="S36:X36"/>
+    <mergeCell ref="L8:Q8"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="S8:X8"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="L36:Q36"/>
-    <mergeCell ref="S36:X36"/>
-    <mergeCell ref="L8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C34">
     <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
@@ -10949,15 +10952,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="str">
@@ -11034,17 +11037,17 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="141"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="129"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -11057,40 +11060,40 @@
     </row>
     <row r="7" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="122" t="s">
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="124"/>
-      <c r="L8" s="122" t="s">
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="134"/>
+      <c r="L8" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="124"/>
-      <c r="S8" s="122" t="s">
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="134"/>
+      <c r="S8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="123"/>
-      <c r="U8" s="123"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="134"/>
     </row>
     <row r="9" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="143"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
@@ -12845,47 +12848,47 @@
       <c r="B36" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="125">
+      <c r="C36" s="135">
         <f>C35+E35</f>
         <v>7.5</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="126"/>
-      <c r="G36" s="127">
+      <c r="D36" s="135"/>
+      <c r="E36" s="136"/>
+      <c r="G36" s="137">
         <f>G35+I35</f>
         <v>10</v>
       </c>
-      <c r="H36" s="128"/>
-      <c r="I36" s="129"/>
-      <c r="L36" s="130">
+      <c r="H36" s="138"/>
+      <c r="I36" s="139"/>
+      <c r="L36" s="140">
         <f>SUM(L35:Q35)</f>
         <v>4.5</v>
       </c>
-      <c r="M36" s="131"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="131"/>
-      <c r="P36" s="131"/>
-      <c r="Q36" s="132"/>
-      <c r="S36" s="133">
+      <c r="M36" s="141"/>
+      <c r="N36" s="141"/>
+      <c r="O36" s="141"/>
+      <c r="P36" s="141"/>
+      <c r="Q36" s="142"/>
+      <c r="S36" s="143">
         <f>SUM(S35:X35)</f>
         <v>6</v>
       </c>
-      <c r="T36" s="134"/>
-      <c r="U36" s="134"/>
-      <c r="V36" s="134"/>
-      <c r="W36" s="134"/>
-      <c r="X36" s="135"/>
+      <c r="T36" s="144"/>
+      <c r="U36" s="144"/>
+      <c r="V36" s="144"/>
+      <c r="W36" s="144"/>
+      <c r="X36" s="145"/>
     </row>
     <row r="37" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="136">
+      <c r="C37" s="124">
         <f>C39*C40</f>
         <v>42</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="137"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
@@ -12933,18 +12936,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S8:X8"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="L36:Q36"/>
+    <mergeCell ref="S36:X36"/>
+    <mergeCell ref="L8:Q8"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="S8:X8"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="L36:Q36"/>
-    <mergeCell ref="S36:X36"/>
-    <mergeCell ref="L8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C34">
     <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThan">
@@ -12991,7 +12994,7 @@
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13009,15 +13012,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="str">
@@ -13094,17 +13097,17 @@
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="140"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
-      <c r="J6" s="141"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="129"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -13117,40 +13120,40 @@
     </row>
     <row r="7" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142" t="s">
+      <c r="B8" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="122" t="s">
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="124"/>
-      <c r="L8" s="122" t="s">
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="134"/>
+      <c r="L8" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="124"/>
-      <c r="S8" s="122" t="s">
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="134"/>
+      <c r="S8" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="123"/>
-      <c r="U8" s="123"/>
-      <c r="V8" s="123"/>
-      <c r="W8" s="123"/>
-      <c r="X8" s="124"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="134"/>
     </row>
     <row r="9" spans="2:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="143"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
@@ -13235,13 +13238,13 @@
       <c r="F10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="165">
+      <c r="G10" s="117">
         <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="164"/>
+      <c r="I10" s="116"/>
       <c r="J10" s="21" t="s">
         <v>71</v>
       </c>
@@ -13317,7 +13320,7 @@
       <c r="H11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="164"/>
+      <c r="I11" s="116"/>
       <c r="J11" s="21" t="s">
         <v>71</v>
       </c>
@@ -13389,7 +13392,7 @@
       <c r="H12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="164"/>
+      <c r="I12" s="116"/>
       <c r="J12" s="21" t="s">
         <v>70</v>
       </c>
@@ -13461,7 +13464,7 @@
       <c r="H13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="164"/>
+      <c r="I13" s="116"/>
       <c r="J13" s="21" t="s">
         <v>68</v>
       </c>
@@ -13533,7 +13536,7 @@
       <c r="H14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="164"/>
+      <c r="I14" s="116"/>
       <c r="J14" s="21" t="s">
         <v>68</v>
       </c>
@@ -13605,7 +13608,7 @@
       <c r="H15" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="164"/>
+      <c r="I15" s="116"/>
       <c r="J15" s="21" t="s">
         <v>69</v>
       </c>
@@ -13677,7 +13680,7 @@
       <c r="H16" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="164"/>
+      <c r="I16" s="116"/>
       <c r="J16" s="21" t="s">
         <v>72</v>
       </c>
@@ -13731,18 +13734,28 @@
       </c>
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
+      <c r="B17" s="16" t="s">
+        <v>102</v>
+      </c>
       <c r="C17" s="20"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="E17" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="G17" s="20"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="I17" s="46"/>
-      <c r="J17" s="21"/>
+      <c r="J17" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="L17" s="40">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -14923,47 +14936,47 @@
       <c r="B36" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="125">
+      <c r="C36" s="135">
         <f>C35+E35</f>
         <v>8.75</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="126"/>
-      <c r="G36" s="127">
+      <c r="D36" s="135"/>
+      <c r="E36" s="136"/>
+      <c r="G36" s="137">
         <f>G35+I35</f>
         <v>7</v>
       </c>
-      <c r="H36" s="128"/>
-      <c r="I36" s="129"/>
-      <c r="L36" s="130">
+      <c r="H36" s="138"/>
+      <c r="I36" s="139"/>
+      <c r="L36" s="140">
         <f>SUM(L35:Q35)</f>
         <v>8.75</v>
       </c>
-      <c r="M36" s="131"/>
-      <c r="N36" s="131"/>
-      <c r="O36" s="131"/>
-      <c r="P36" s="131"/>
-      <c r="Q36" s="132"/>
-      <c r="S36" s="133">
+      <c r="M36" s="141"/>
+      <c r="N36" s="141"/>
+      <c r="O36" s="141"/>
+      <c r="P36" s="141"/>
+      <c r="Q36" s="142"/>
+      <c r="S36" s="143">
         <f>SUM(S35:X35)</f>
         <v>7</v>
       </c>
-      <c r="T36" s="134"/>
-      <c r="U36" s="134"/>
-      <c r="V36" s="134"/>
-      <c r="W36" s="134"/>
-      <c r="X36" s="135"/>
+      <c r="T36" s="144"/>
+      <c r="U36" s="144"/>
+      <c r="V36" s="144"/>
+      <c r="W36" s="144"/>
+      <c r="X36" s="145"/>
     </row>
     <row r="37" spans="2:24" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="136">
+      <c r="C37" s="124">
         <f>C39*C40</f>
         <v>42</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="137"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
@@ -15011,18 +15024,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="S8:X8"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="L36:Q36"/>
+    <mergeCell ref="S36:X36"/>
+    <mergeCell ref="L8:Q8"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
-    <mergeCell ref="S8:X8"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="L36:Q36"/>
-    <mergeCell ref="S36:X36"/>
-    <mergeCell ref="L8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:C34">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
@@ -15067,9 +15080,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15276,27 +15292,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21F7B50A-2E98-44F9-ACD4-50B4039AFCBB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19769AF-35A5-453C-B678-4E12F267A32D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a24e9797-c9de-4ae0-9124-5b215385d802"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="85fa55d4-3ee8-4bc4-8fbc-63473e847397"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15321,9 +15325,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19769AF-35A5-453C-B678-4E12F267A32D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21F7B50A-2E98-44F9-ACD4-50B4039AFCBB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a24e9797-c9de-4ae0-9124-5b215385d802"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="85fa55d4-3ee8-4bc4-8fbc-63473e847397"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>